<commit_message>
read message field in holvi import file too
</commit_message>
<xml_diff>
--- a/utils/holvi-account-test-statement-2022-10.xlsx
+++ b/utils/holvi-account-test-statement-2022-10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t xml:space="preserve">IBAN</t>
   </si>
@@ -179,6 +179,39 @@
   </si>
   <si>
     <t xml:space="preserve">1924ceba5a3b1c5ffea892fb4850e00a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Sept 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test without either reference or message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1924ceba5a3b1c5ffea892fb4850e00b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Sept 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test without reference and with message that is not reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1924ceba5a3b1c5ffea892fb4850e00c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Sept 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test without reference and with message that has the reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000200047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1924ceba5a3b1c5ffea892fb4850e00d</t>
   </si>
 </sst>
 </file>
@@ -254,8 +287,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,321 +313,394 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>718</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>2083.34</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>-135.9</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>1122002246684</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>201333</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="0" t="n">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>-7.44</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -597,10 +711,11 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>

<commit_message>
Get reference also from transaction message (#530)
* Get reference also from message

* read message field in holvi import file too

* blackened
</commit_message>
<xml_diff>
--- a/utils/holvi-account-test-statement-2022-10.xlsx
+++ b/utils/holvi-account-test-statement-2022-10.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="64">
   <si>
     <t xml:space="preserve">IBAN</t>
   </si>
@@ -179,6 +179,39 @@
   </si>
   <si>
     <t xml:space="preserve">1924ceba5a3b1c5ffea892fb4850e00a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2 Sept 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test without either reference or message</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1924ceba5a3b1c5ffea892fb4850e00b</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3 Sept 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test without reference and with message that is not reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1924ceba5a3b1c5ffea892fb4850e00c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4 Sept 2022</t>
+  </si>
+  <si>
+    <t xml:space="preserve">test without reference and with message that has the reference</t>
+  </si>
+  <si>
+    <t xml:space="preserve">00000200047</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1924ceba5a3b1c5ffea892fb4850e00d</t>
   </si>
 </sst>
 </file>
@@ -254,8 +287,16 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -272,321 +313,394 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I29"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I20" activeCellId="0" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="24"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="9"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="31"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="21"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="9"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="53"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="33"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="1" t="n">
         <v>718</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="1" t="n">
         <v>6</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="0" t="n">
+      <c r="B6" s="1" t="n">
         <v>2083.34</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="1" t="n">
         <v>2</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="C8" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D8" s="0" t="s">
+      <c r="D8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="E8" s="0" t="s">
+      <c r="E8" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="F8" s="0" t="s">
+      <c r="F8" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="G8" s="0" t="s">
+      <c r="G8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="0" t="s">
+      <c r="H8" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="I8" s="0" t="s">
+      <c r="I8" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C9" s="0" t="n">
+      <c r="B9" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="1" t="n">
         <v>-135.9</v>
       </c>
-      <c r="D9" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="0" t="s">
+      <c r="D9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="0" t="s">
+      <c r="F9" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="G9" s="0" t="n">
+      <c r="G9" s="1" t="n">
         <v>1122002246684</v>
       </c>
-      <c r="I9" s="0" t="s">
+      <c r="I9" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B10" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C10" s="0" t="n">
+      <c r="A10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D10" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="0" t="s">
+      <c r="D10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="0" t="s">
+      <c r="F10" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="G10" s="0" t="n">
+      <c r="G10" s="1" t="n">
         <v>201333</v>
       </c>
-      <c r="I10" s="0" t="s">
+      <c r="I10" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="0" t="n">
+      <c r="A11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D11" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E11" s="0" t="s">
+      <c r="D11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="F11" s="0" t="s">
+      <c r="F11" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="G11" s="0" t="s">
+      <c r="G11" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="I11" s="0" t="s">
+      <c r="I11" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B12" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="0" t="n">
-        <v>20</v>
-      </c>
-      <c r="D12" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E12" s="0" t="s">
+      <c r="A12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="1" t="n">
+        <v>20</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F12" s="0" t="s">
+      <c r="F12" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="0" t="s">
+      <c r="G12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I12" s="0" t="s">
+      <c r="I12" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="C13" s="0" t="n">
+      <c r="A13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C13" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="D13" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="0" t="s">
+      <c r="D13" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F13" s="0" t="s">
+      <c r="F13" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G13" s="0" t="s">
+      <c r="G13" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="I13" s="0" t="s">
+      <c r="I13" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="B14" s="0" t="s">
+      <c r="B14" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="D14" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E14" s="0" t="s">
+      <c r="D14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="F14" s="0" t="s">
+      <c r="F14" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="G14" s="0" t="s">
+      <c r="G14" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I14" s="0" t="s">
+      <c r="I14" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B15" s="0" t="s">
+      <c r="B15" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="C15" s="1" t="n">
         <v>-7.44</v>
       </c>
-      <c r="D15" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E15" s="0" t="s">
+      <c r="D15" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E15" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="0" t="s">
+      <c r="F15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="G15" s="0" t="s">
+      <c r="G15" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="I15" s="0" t="s">
+      <c r="I15" s="1" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="14.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B16" s="0" t="s">
+      <c r="B16" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="C16" s="1" t="n">
         <v>30</v>
       </c>
-      <c r="D16" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="E16" s="0" t="s">
+      <c r="D16" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E16" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="F16" s="0" t="s">
+      <c r="F16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="G16" s="0" t="s">
+      <c r="G16" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="I16" s="0" t="s">
+      <c r="I16" s="1" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C17" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C18" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="I18" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C19" s="1" t="n">
+        <v>30</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I19" s="1" t="s">
+        <v>63</v>
+      </c>
+    </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -597,10 +711,11 @@
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader/>
     <oddFooter/>

</xml_diff>